<commit_message>
marker column somehow removed and I added them back
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_480.xlsx
+++ b/bioSample/bioSample_480.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C217E56F-FFCF-4C40-BF59-C47EF62F921E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0588526-7469-1446-B7EB-4535547B1826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4880" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bioSample_480" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
   <si>
     <t>harvestDate</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>TDY1145</t>
+  </si>
+  <si>
+    <t>marker_1</t>
+  </si>
+  <si>
+    <t>marker_2</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -452,7 +458,7 @@
     <col min="10" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +486,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -510,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -539,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -568,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -597,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -626,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -655,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -684,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -713,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -742,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -771,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -800,7 +812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>9</v>
       </c>

</xml_diff>